<commit_message>
in schematic transistor switching,side leds added right angle connector s added
in schematic transistor switching logic, side leds added ,right angle
connector s added
</commit_message>
<xml_diff>
--- a/thingTouch-Buttons/v1.0/thingTouch-Buttons_v1P0.xlsx
+++ b/thingTouch-Buttons/v1.0/thingTouch-Buttons_v1P0.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="thingTouch-Buttons_v1P0" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -1098,7 +1098,7 @@
   <dimension ref="A1:Q13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Gerbers generated, design verified
Gerbers generated, design verified
</commit_message>
<xml_diff>
--- a/thingTouch-Buttons/v1.0/thingTouch-Buttons_v1P0.xlsx
+++ b/thingTouch-Buttons/v1.0/thingTouch-Buttons_v1P0.xlsx
@@ -725,7 +725,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -742,7 +742,6 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -753,6 +752,15 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1098,7 +1106,7 @@
   <dimension ref="A1:Q13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1181,7 +1189,7 @@
       <c r="F2" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="9" t="s">
         <v>52</v>
       </c>
       <c r="H2" s="7">
@@ -1190,16 +1198,16 @@
       <c r="I2" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="11">
+      <c r="J2" s="10">
         <v>7.7</v>
       </c>
-      <c r="K2" s="11">
+      <c r="K2" s="10">
         <v>2.8</v>
       </c>
-      <c r="L2" s="11">
+      <c r="L2" s="10">
         <v>2.8</v>
       </c>
-      <c r="M2" s="11">
+      <c r="M2" s="10">
         <v>2.59</v>
       </c>
       <c r="O2">
@@ -1231,7 +1239,7 @@
       <c r="F3" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="9" t="s">
         <v>52</v>
       </c>
       <c r="H3" s="7">
@@ -1240,16 +1248,16 @@
       <c r="I3" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="11">
+      <c r="J3" s="10">
         <v>7.7</v>
       </c>
-      <c r="K3" s="11">
+      <c r="K3" s="10">
         <v>2.8</v>
       </c>
-      <c r="L3" s="11">
+      <c r="L3" s="10">
         <v>2.8</v>
       </c>
-      <c r="M3" s="11">
+      <c r="M3" s="10">
         <v>2.59</v>
       </c>
       <c r="O3">
@@ -1281,7 +1289,7 @@
       <c r="F4" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="G4" s="9" t="s">
         <v>52</v>
       </c>
       <c r="H4" s="7">
@@ -1290,16 +1298,16 @@
       <c r="I4" t="s">
         <v>3</v>
       </c>
-      <c r="J4" s="11">
+      <c r="J4" s="10">
         <v>7.7</v>
       </c>
-      <c r="K4" s="11">
+      <c r="K4" s="10">
         <v>2.8</v>
       </c>
-      <c r="L4" s="11">
+      <c r="L4" s="10">
         <v>2.8</v>
       </c>
-      <c r="M4" s="11">
+      <c r="M4" s="10">
         <v>2.59</v>
       </c>
       <c r="O4">
@@ -1315,81 +1323,81 @@
         <v>2.59</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5">
+    <row r="5" spans="1:17" s="12" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="12">
         <v>1</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="H5" s="9">
+      <c r="H5" s="16">
         <v>805</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" s="12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6">
+    <row r="6" spans="1:17" s="12" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="12">
         <v>1</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="G6" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="H6" s="9">
+      <c r="H6" s="16">
         <v>805</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" s="12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7">
+    <row r="7" spans="1:17" s="12" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="12">
         <v>1</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="G7" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="H7" s="9">
+      <c r="H7" s="16">
         <v>805</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I7" s="12" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1440,22 +1448,22 @@
       <c r="G10" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="H10" s="9">
+      <c r="H10" s="8">
         <v>805</v>
       </c>
       <c r="I10" t="s">
         <v>23</v>
       </c>
-      <c r="J10" s="11">
+      <c r="J10" s="10">
         <v>7.7</v>
       </c>
-      <c r="K10" s="11">
+      <c r="K10" s="10">
         <v>2.8</v>
       </c>
-      <c r="L10" s="11">
+      <c r="L10" s="10">
         <v>2.8</v>
       </c>
-      <c r="M10" s="11">
+      <c r="M10" s="10">
         <v>2.59</v>
       </c>
       <c r="O10">
@@ -1490,22 +1498,22 @@
       <c r="G11" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="H11" s="9">
+      <c r="H11" s="8">
         <v>805</v>
       </c>
       <c r="I11" t="s">
         <v>23</v>
       </c>
-      <c r="J11" s="11">
+      <c r="J11" s="10">
         <v>7.7</v>
       </c>
-      <c r="K11" s="11">
+      <c r="K11" s="10">
         <v>2.8</v>
       </c>
-      <c r="L11" s="11">
+      <c r="L11" s="10">
         <v>2.8</v>
       </c>
-      <c r="M11" s="11">
+      <c r="M11" s="10">
         <v>2.59</v>
       </c>
       <c r="O11">
@@ -1535,20 +1543,20 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="12">
+    <row r="13" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="11">
         <v>3</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="D13" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="E13" s="12" t="s">
+      <c r="E13" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="I13" s="12" t="s">
+      <c r="I13" s="11" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>